<commit_message>
Se agregan los scripts de generación de tablas de hechos y dimensiones
</commit_message>
<xml_diff>
--- a/practicas/diseno_dimensional.xlsx
+++ b/practicas/diseno_dimensional.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="160">
-  <si>
-    <t>dim_clasificador_entidades</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="160">
+  <si>
+    <t>dim_clasificador_entidad</t>
   </si>
   <si>
     <t>dim_clasificador_funcion</t>
@@ -123,264 +123,264 @@
     <t>funcion_descripcion</t>
   </si>
   <si>
+    <t>clasificador_geografico</t>
+  </si>
+  <si>
+    <t>junk_contrato</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>numeric(1,0)</t>
+  </si>
+  <si>
+    <t>unidad_jerarquica_codigo</t>
+  </si>
+  <si>
+    <t>subfuncion_codigo</t>
+  </si>
+  <si>
+    <t>clasificador_control_financiero</t>
+  </si>
+  <si>
+    <t>id_llamado</t>
+  </si>
+  <si>
+    <t>checksum</t>
+  </si>
+  <si>
+    <t>character varying</t>
+  </si>
+  <si>
+    <t>unidad_jerarquica_descripcion</t>
+  </si>
+  <si>
+    <t>subfuncion_descripcion</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>clasificador_entidad_destino</t>
+  </si>
+  <si>
+    <t>codigo_contratacion</t>
+  </si>
+  <si>
+    <t>uaf_codigo</t>
+  </si>
+  <si>
+    <t>fecha_generacion</t>
+  </si>
+  <si>
+    <t>monto_adjudicado</t>
+  </si>
+  <si>
+    <t>dim_tipo_procedimiento_dncp</t>
+  </si>
+  <si>
+    <t>uaf_descripcion</t>
+  </si>
+  <si>
+    <t>fecha_recepcion_tesoro</t>
+  </si>
+  <si>
+    <t>fecha_deposito</t>
+  </si>
+  <si>
+    <t>unidad_responsable_codigo</t>
+  </si>
+  <si>
+    <t>dim_junk_contrato</t>
+  </si>
+  <si>
+    <t>tipo_procedimiento_codigo</t>
+  </si>
+  <si>
+    <t>unidad_responsable_descripcion</t>
+  </si>
+  <si>
+    <t>junk_str</t>
+  </si>
+  <si>
+    <t>cuenta_origen</t>
+  </si>
+  <si>
+    <t>tipo_procedimiento_descripcion</t>
+  </si>
+  <si>
+    <t>junk_obligacion</t>
+  </si>
+  <si>
+    <t>cuenta_destino</t>
+  </si>
+  <si>
+    <t>nombre_licitacion</t>
+  </si>
+  <si>
+    <t>dim_clasificador_fuente_financiamiento</t>
+  </si>
+  <si>
+    <t>numero_obligacion</t>
+  </si>
+  <si>
+    <t>numero_str</t>
+  </si>
+  <si>
+    <t>junk_ot</t>
+  </si>
+  <si>
+    <t>convocante</t>
+  </si>
+  <si>
+    <t>monto_solicitado</t>
+  </si>
+  <si>
+    <t>numero_ot</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>monto_obligado</t>
+  </si>
+  <si>
+    <t>monto_deducciones</t>
+  </si>
+  <si>
+    <t>moneda_codigo</t>
+  </si>
+  <si>
+    <t>fuente_financiamiento_codigo</t>
+  </si>
+  <si>
+    <t>monto_deduccion_iva</t>
+  </si>
+  <si>
+    <t>cotizacion</t>
+  </si>
+  <si>
+    <t>moneda_simbolo</t>
+  </si>
+  <si>
+    <t>dim_clasificador_programa</t>
+  </si>
+  <si>
+    <t>fuente_financiamiento_descripcion</t>
+  </si>
+  <si>
+    <t>monto_deduccion_renta</t>
+  </si>
+  <si>
+    <t>dim_junk_str</t>
+  </si>
+  <si>
+    <t>monto_ot</t>
+  </si>
+  <si>
+    <t>moneda_descripcion</t>
+  </si>
+  <si>
+    <t>organismo_financiador_codigo</t>
+  </si>
+  <si>
+    <t>monto_deduccion_dncp</t>
+  </si>
+  <si>
+    <t>monto_ot_gs</t>
+  </si>
+  <si>
+    <t>vigencia_contrato</t>
+  </si>
+  <si>
+    <t>organismo_financiador_descripcion</t>
+  </si>
+  <si>
+    <t>monto_deduccion_incumplimiento_contrato</t>
+  </si>
+  <si>
+    <t>situacion_str_codigo</t>
+  </si>
+  <si>
+    <t>monto_ot_destino</t>
+  </si>
+  <si>
+    <t>tipo_presupuesto_codigo</t>
+  </si>
+  <si>
+    <t>monto_deduccion_otras</t>
+  </si>
+  <si>
+    <t>situacion_str_descripcion</t>
+  </si>
+  <si>
+    <t>tipo_presupuesto_descripcion</t>
+  </si>
+  <si>
+    <t>tipo_str_codigo</t>
+  </si>
+  <si>
+    <t>dim_junk_ot</t>
+  </si>
+  <si>
+    <t>programa_codigo</t>
+  </si>
+  <si>
+    <t>dim_junk_obligacion</t>
+  </si>
+  <si>
+    <t>tipo_str_descripcion</t>
+  </si>
+  <si>
+    <t>programa_descripcion</t>
+  </si>
+  <si>
+    <t>descripcion_str</t>
+  </si>
+  <si>
+    <t>concepto_codigo</t>
+  </si>
+  <si>
+    <t>subprograma_codigo</t>
+  </si>
+  <si>
+    <t>concepto_obligacion_codigo</t>
+  </si>
+  <si>
+    <t>detalle_str</t>
+  </si>
+  <si>
+    <t>concepto_descripcion</t>
+  </si>
+  <si>
+    <t>br_obligacion_contrato</t>
+  </si>
+  <si>
+    <t>subprograma_descripcion</t>
+  </si>
+  <si>
+    <t>dim_clasificador_geografico</t>
+  </si>
+  <si>
+    <t>concepto_obligacion_descripcion</t>
+  </si>
+  <si>
+    <t>proyecto_codigo</t>
+  </si>
+  <si>
+    <t>obligacion</t>
+  </si>
+  <si>
+    <t>proyecto_descripcion</t>
+  </si>
+  <si>
+    <t>pais_codigo</t>
+  </si>
+  <si>
     <t>contrato</t>
   </si>
   <si>
-    <t>clasificador_geografico</t>
-  </si>
-  <si>
-    <t>junk_contrato</t>
-  </si>
-  <si>
-    <t>actual</t>
-  </si>
-  <si>
-    <t>numeric(1,0)</t>
-  </si>
-  <si>
-    <t>unidad_jerarquica_codigo</t>
-  </si>
-  <si>
-    <t>subfuncion_codigo</t>
-  </si>
-  <si>
-    <t>clasificador_control_financiero</t>
-  </si>
-  <si>
-    <t>id_llamado</t>
-  </si>
-  <si>
-    <t>checksum</t>
-  </si>
-  <si>
-    <t>character varying</t>
-  </si>
-  <si>
-    <t>unidad_jerarquica_descripcion</t>
-  </si>
-  <si>
-    <t>subfuncion_descripcion</t>
-  </si>
-  <si>
-    <t>fecha_ingreso</t>
-  </si>
-  <si>
-    <t>clasificador_entidad_destino</t>
-  </si>
-  <si>
-    <t>codigo_contratacion</t>
-  </si>
-  <si>
-    <t>uaf_codigo</t>
-  </si>
-  <si>
-    <t>fecha_generacion</t>
-  </si>
-  <si>
-    <t>monto_adjudicado</t>
-  </si>
-  <si>
-    <t>dim_tipo_procedimiento_dncp</t>
-  </si>
-  <si>
-    <t>uaf_descripcion</t>
-  </si>
-  <si>
-    <t>fecha_recepcion_tesoro</t>
-  </si>
-  <si>
-    <t>fecha_deposito</t>
-  </si>
-  <si>
-    <t>unidad_responsable_codigo</t>
-  </si>
-  <si>
-    <t>dim_junk_contrato</t>
-  </si>
-  <si>
-    <t>tipo_procedimiento_codigo</t>
-  </si>
-  <si>
-    <t>unidad_responsable_descripcion</t>
-  </si>
-  <si>
-    <t>junk_str</t>
-  </si>
-  <si>
-    <t>cuenta_origen</t>
-  </si>
-  <si>
-    <t>tipo_procedimiento_descripcion</t>
-  </si>
-  <si>
-    <t>junk_obligacion</t>
-  </si>
-  <si>
-    <t>cuenta_destino</t>
-  </si>
-  <si>
-    <t>nombre_licitacion</t>
-  </si>
-  <si>
-    <t>dim_clasificador_fuente_financiamiento</t>
-  </si>
-  <si>
-    <t>numero_obligacion</t>
-  </si>
-  <si>
-    <t>numero_str</t>
-  </si>
-  <si>
-    <t>junk_ot</t>
-  </si>
-  <si>
-    <t>convocante</t>
-  </si>
-  <si>
-    <t>monto_solicitado</t>
-  </si>
-  <si>
-    <t>numero_ot</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>monto_obligado</t>
-  </si>
-  <si>
-    <t>monto_deducciones</t>
-  </si>
-  <si>
-    <t>moneda_codigo</t>
-  </si>
-  <si>
-    <t>fuente_financiamiento_codigo</t>
-  </si>
-  <si>
-    <t>monto_deduccion_iva</t>
-  </si>
-  <si>
-    <t>cotizacion</t>
-  </si>
-  <si>
-    <t>moneda_simbolo</t>
-  </si>
-  <si>
-    <t>dim_clasificador_programa</t>
-  </si>
-  <si>
-    <t>fuente_financiamiento_descripcion</t>
-  </si>
-  <si>
-    <t>monto_deduccion_renta</t>
-  </si>
-  <si>
-    <t>dim_junk_str</t>
-  </si>
-  <si>
-    <t>monto_ot</t>
-  </si>
-  <si>
-    <t>moneda_descripcion</t>
-  </si>
-  <si>
-    <t>organismo_financiador_codigo</t>
-  </si>
-  <si>
-    <t>monto_deduccion_dncp</t>
-  </si>
-  <si>
-    <t>monto_ot_gs</t>
-  </si>
-  <si>
-    <t>vigencia_contrato</t>
-  </si>
-  <si>
-    <t>organismo_financiador_descripcion</t>
-  </si>
-  <si>
-    <t>monto_deduccion_incumplimiento_contrato</t>
-  </si>
-  <si>
-    <t>situacion_str_codigo</t>
-  </si>
-  <si>
-    <t>monto_ot_destino</t>
-  </si>
-  <si>
-    <t>tipo_presupuesto_codigo</t>
-  </si>
-  <si>
-    <t>monto_deduccion_otras</t>
-  </si>
-  <si>
-    <t>situacion_str_descripcion</t>
-  </si>
-  <si>
-    <t>tipo_presupuesto_descripcion</t>
-  </si>
-  <si>
-    <t>tipo_str_codigo</t>
-  </si>
-  <si>
-    <t>dim_junk_ot</t>
-  </si>
-  <si>
-    <t>programa_codigo</t>
-  </si>
-  <si>
-    <t>dim_junk_obligacion</t>
-  </si>
-  <si>
-    <t>tipo_str_descripcion</t>
-  </si>
-  <si>
-    <t>programa_descripcion</t>
-  </si>
-  <si>
-    <t>descripcion_str</t>
-  </si>
-  <si>
-    <t>concepto_codigo</t>
-  </si>
-  <si>
-    <t>subprograma_codigo</t>
-  </si>
-  <si>
-    <t>concepto_obligacion_codigo</t>
-  </si>
-  <si>
-    <t>detalle_str</t>
-  </si>
-  <si>
-    <t>concepto_descripcion</t>
-  </si>
-  <si>
-    <t>br_obligacion_contrato</t>
-  </si>
-  <si>
-    <t>subprograma_descripcion</t>
-  </si>
-  <si>
-    <t>dim_clasificador_geografico</t>
-  </si>
-  <si>
-    <t>concepto_obligacion_descripcion</t>
-  </si>
-  <si>
-    <t>proyecto_codigo</t>
-  </si>
-  <si>
-    <t>obligacion</t>
-  </si>
-  <si>
-    <t>proyecto_descripcion</t>
-  </si>
-  <si>
-    <t>pais_codigo</t>
-  </si>
-  <si>
     <t>pais_simbolo</t>
   </si>
   <si>
@@ -453,7 +453,7 @@
     <t>control_financiero_descripcion</t>
   </si>
   <si>
-    <t>dim_cuentas_bancarias</t>
+    <t>dim_cuenta_bancaria</t>
   </si>
   <si>
     <t>banco_codigo</t>
@@ -465,7 +465,7 @@
     <t>dim_tiempo</t>
   </si>
   <si>
-    <t>banco_abreviatura</t>
+    <t>banco_simbolo</t>
   </si>
   <si>
     <t>numero_cuenta</t>
@@ -474,13 +474,13 @@
     <t>Codigos</t>
   </si>
   <si>
-    <t>numeric(5,0)</t>
+    <t>Numeric(5,0)</t>
   </si>
   <si>
     <t>Montos</t>
   </si>
   <si>
-    <t>numeric(15,2)</t>
+    <t>Numeric(17,2)</t>
   </si>
   <si>
     <t>Descripciones</t>
@@ -495,7 +495,7 @@
     <t>Numeros Enteros</t>
   </si>
   <si>
-    <t>numeric(13,0)</t>
+    <t>Numeric(7,0)</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -533,11 +533,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -588,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,19 +596,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,10 +621,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -649,19 +636,22 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9285714285714"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8418367346939"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.5867346938775"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="28.8979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.8979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7142857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9336734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="28.8979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.9642857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3367346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.8979591836735"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.7142857142857"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6275510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.0867346938776"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3826530612245"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.7142857142857"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.6275510204082"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="23.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +661,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="str">
         <f aca="false">"CREATE TABLE "&amp;A1&amp;" ("</f>
-        <v>CREATE TABLE dim_clasificador_entidades (</v>
+        <v>CREATE TABLE dim_clasificador_entidad (</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -689,35 +679,39 @@
         <f aca="false">"CREATE TABLE "&amp;G1&amp;" ("</f>
         <v>CREATE TABLE fact_obligacion (</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;J1&amp;" ("</f>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;K1&amp;" ("</f>
         <v>CREATE TABLE fact_str (</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;M1&amp;" ("</f>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;O1&amp;" ("</f>
         <v>CREATE TABLE fact_ot (</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="2"/>
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;P1&amp;" ("</f>
-        <v>CREATE TABLE fact_contrato (</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="T1" s="1"/>
       <c r="U1" s="2" t="str">
         <f aca="false">"CREATE TABLE "&amp;S1&amp;" ("</f>
+        <v>CREATE TABLE fact_contrato (</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="W1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;W1&amp;" ("</f>
         <v>CREATE TABLE dim_categoria_dncp (</v>
       </c>
     </row>
@@ -752,34 +746,24 @@
         <f aca="false">G2&amp;" "&amp;H2&amp;","</f>
         <v>id bigserial,</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="0" t="str">
-        <f aca="false">J2&amp;" "&amp;K2&amp;","</f>
+      <c r="M2" s="0" t="str">
+        <f aca="false">K2&amp;" "&amp;L2&amp;","</f>
         <v>id bigserial,</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="0" t="str">
-        <f aca="false">M2&amp;" "&amp;N2&amp;","</f>
-        <v>id bigserial,</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="0" t="str">
-        <f aca="false">P2&amp;" "&amp;Q2&amp;","</f>
+      <c r="Q2" s="0" t="str">
+        <f aca="false">O2&amp;" "&amp;P2&amp;","</f>
         <v>id bigserial,</v>
       </c>
       <c r="S2" s="0" t="s">
@@ -792,6 +776,16 @@
         <f aca="false">S2&amp;" "&amp;T2&amp;","</f>
         <v>id bigserial,</v>
       </c>
+      <c r="W2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="0" t="str">
+        <f aca="false">W2&amp;" "&amp;X2&amp;","</f>
+        <v>id bigserial,</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -825,49 +819,65 @@
         <f aca="false">G3&amp;" "&amp;H3&amp;","</f>
         <v>fecha_elaboracion bigint,</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G3&amp;" FOREIGN KEY ("&amp;G3&amp;") REFERENCES "&amp;IF(LEFT(G3,5)="fecha","dim_tiempo",IF(LEFT(G3,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G3))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_elaboracion FOREIGN KEY (fecha_elaboracion) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L3" s="0" t="str">
-        <f aca="false">J3&amp;" "&amp;K3&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">K3&amp;" "&amp;L3&amp;","</f>
         <v>clasificador_entidad bigint,</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="N3" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K3&amp;" FOREIGN KEY ("&amp;K3&amp;") REFERENCES "&amp;IF(LEFT(K3,5)="fecha","dim_tiempo",IF(LEFT(K3,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K3))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_entidad FOREIGN KEY (clasificador_entidad) REFERENCES dim_clasificador_entidad(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O3" s="0" t="str">
-        <f aca="false">M3&amp;" "&amp;N3&amp;","</f>
+      <c r="P3" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q3" s="0" t="str">
+        <f aca="false">O3&amp;" "&amp;P3&amp;","</f>
         <v>clasificador_entidad bigint,</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="R3" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O3&amp;" FOREIGN KEY ("&amp;O3&amp;") REFERENCES "&amp;IF(LEFT(O3,5)="fecha","dim_tiempo",IF(LEFT(O3,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O3))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_entidad FOREIGN KEY (clasificador_entidad) REFERENCES dim_clasificador_entidad(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R3" s="0" t="str">
-        <f aca="false">P3&amp;" "&amp;Q3&amp;","</f>
-        <v>categoria_dncp bigint,</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="T3" s="0" t="str">
-        <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
       </c>
       <c r="U3" s="0" t="str">
         <f aca="false">S3&amp;" "&amp;T3&amp;","</f>
-        <v>categoria_codigo numeric(5,0),</v>
+        <v>categoria_dncp bigint,</v>
+      </c>
+      <c r="V3" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;S3&amp;" FOREIGN KEY ("&amp;S3&amp;") REFERENCES "&amp;IF(LEFT(S3,5)="fecha","dim_tiempo",IF(LEFT(S3,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;S3))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_categoria_dncp FOREIGN KEY (categoria_dncp) REFERENCES dim_categoria_dncp(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="0" t="str">
+        <f aca="false">Sheet2!$B$1</f>
+        <v>Numeric(5,0)</v>
+      </c>
+      <c r="Y3" s="0" t="str">
+        <f aca="false">W3&amp;" "&amp;X3&amp;","</f>
+        <v>categoria_codigo Numeric(5,0),</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,22 +886,22 @@
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A4&amp;" "&amp;B4&amp;","</f>
-        <v>nivel_codigo numeric(5,0),</v>
+        <v>nivel_codigo Numeric(5,0),</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">D4&amp;" "&amp;E4&amp;","</f>
-        <v>finalidad_codigo numeric(5,0),</v>
+        <v>finalidad_codigo Numeric(5,0),</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>17</v>
@@ -904,48 +914,64 @@
         <f aca="false">G4&amp;" "&amp;H4&amp;","</f>
         <v>fecha_aprobacion bigint,</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G4&amp;" FOREIGN KEY ("&amp;G4&amp;") REFERENCES "&amp;IF(LEFT(G4,5)="fecha","dim_tiempo",IF(LEFT(G4,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G4))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_aprobacion FOREIGN KEY (fecha_aprobacion) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L4" s="0" t="str">
-        <f aca="false">J4&amp;" "&amp;K4&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">K4&amp;" "&amp;L4&amp;","</f>
         <v>clasificador_programa bigint,</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K4&amp;" FOREIGN KEY ("&amp;K4&amp;") REFERENCES "&amp;IF(LEFT(K4,5)="fecha","dim_tiempo",IF(LEFT(K4,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K4))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_programa FOREIGN KEY (clasificador_programa) REFERENCES dim_clasificador_programa(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O4" s="0" t="str">
-        <f aca="false">M4&amp;" "&amp;N4&amp;","</f>
+      <c r="P4" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q4" s="0" t="str">
+        <f aca="false">O4&amp;" "&amp;P4&amp;","</f>
         <v>clasificador_programa bigint,</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="R4" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O4&amp;" FOREIGN KEY ("&amp;O4&amp;") REFERENCES "&amp;IF(LEFT(O4,5)="fecha","dim_tiempo",IF(LEFT(O4,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O4))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_programa FOREIGN KEY (clasificador_programa) REFERENCES dim_clasificador_programa(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R4" s="0" t="str">
-        <f aca="false">P4&amp;" "&amp;Q4&amp;","</f>
-        <v>tipo_procedimiento_dncp bigint,</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="T4" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
       </c>
       <c r="U4" s="0" t="str">
         <f aca="false">S4&amp;" "&amp;T4&amp;","</f>
+        <v>tipo_procedimiento_dncp bigint,</v>
+      </c>
+      <c r="V4" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;S4&amp;" FOREIGN KEY ("&amp;S4&amp;") REFERENCES "&amp;IF(LEFT(S4,5)="fecha","dim_tiempo",IF(LEFT(S4,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;S4))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_tipo_procedimiento_dncp FOREIGN KEY (tipo_procedimiento_dncp) REFERENCES dim_tipo_procedimiento_dncp(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="Y4" s="0" t="str">
+        <f aca="false">W4&amp;" "&amp;X4&amp;","</f>
         <v>categoria_descripcion character varying,</v>
       </c>
     </row>
@@ -983,47 +1009,63 @@
         <f aca="false">G5&amp;" "&amp;H5&amp;","</f>
         <v>proveedor bigint,</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G5&amp;" FOREIGN KEY ("&amp;G5&amp;") REFERENCES "&amp;IF(LEFT(G5,5)="fecha","dim_tiempo",IF(LEFT(G5,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G5))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_proveedor FOREIGN KEY (proveedor) REFERENCES dim_proveedor(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="4" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L5" s="0" t="str">
-        <f aca="false">J5&amp;" "&amp;K5&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">K5&amp;" "&amp;L5&amp;","</f>
         <v>clasificador_objeto_gasto bigint,</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="N5" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K5&amp;" FOREIGN KEY ("&amp;K5&amp;") REFERENCES "&amp;IF(LEFT(K5,5)="fecha","dim_tiempo",IF(LEFT(K5,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K5))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_objeto_gasto FOREIGN KEY (clasificador_objeto_gasto) REFERENCES dim_clasificador_objeto_gasto(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O5" s="0" t="str">
-        <f aca="false">M5&amp;" "&amp;N5&amp;","</f>
+      <c r="P5" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q5" s="0" t="str">
+        <f aca="false">O5&amp;" "&amp;P5&amp;","</f>
         <v>clasificador_objeto_gasto bigint,</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="R5" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O5&amp;" FOREIGN KEY ("&amp;O5&amp;") REFERENCES "&amp;IF(LEFT(O5,5)="fecha","dim_tiempo",IF(LEFT(O5,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O5))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_objeto_gasto FOREIGN KEY (clasificador_objeto_gasto) REFERENCES dim_clasificador_objeto_gasto(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R5" s="0" t="str">
-        <f aca="false">P5&amp;" "&amp;Q5&amp;","</f>
-        <v>proveedor bigint,</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>26</v>
+      <c r="T5" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
       </c>
       <c r="U5" s="0" t="str">
         <f aca="false">S5&amp;" "&amp;T5&amp;","</f>
+        <v>proveedor bigint,</v>
+      </c>
+      <c r="V5" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;S5&amp;" FOREIGN KEY ("&amp;S5&amp;") REFERENCES "&amp;IF(LEFT(S5,5)="fecha","dim_tiempo",IF(LEFT(S5,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;S5))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_proveedor FOREIGN KEY (proveedor) REFERENCES dim_proveedor(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="0" t="str">
+        <f aca="false">W5&amp;" "&amp;X5&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
     </row>
@@ -1033,22 +1075,22 @@
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">A6&amp;" "&amp;B6&amp;","</f>
-        <v>entidad_codigo numeric(5,0),</v>
+        <v>entidad_codigo Numeric(5,0),</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F6" s="0" t="str">
         <f aca="false">D6&amp;" "&amp;E6&amp;","</f>
-        <v>funcion_codigo numeric(5,0),</v>
+        <v>funcion_codigo Numeric(5,0),</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>29</v>
@@ -1061,47 +1103,63 @@
         <f aca="false">G6&amp;" "&amp;H6&amp;","</f>
         <v>fecha_factura bigint,</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G6&amp;" FOREIGN KEY ("&amp;G6&amp;") REFERENCES "&amp;IF(LEFT(G6,5)="fecha","dim_tiempo",IF(LEFT(G6,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G6))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_factura FOREIGN KEY (fecha_factura) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L6" s="0" t="str">
-        <f aca="false">J6&amp;" "&amp;K6&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">K6&amp;" "&amp;L6&amp;","</f>
         <v>clasificador_fuente_financiamiento bigint,</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="N6" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K6&amp;" FOREIGN KEY ("&amp;K6&amp;") REFERENCES "&amp;IF(LEFT(K6,5)="fecha","dim_tiempo",IF(LEFT(K6,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K6))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_fuente_financiamiento FOREIGN KEY (clasificador_fuente_financiamiento) REFERENCES dim_clasificador_fuente_financiamiento(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O6" s="0" t="str">
-        <f aca="false">M6&amp;" "&amp;N6&amp;","</f>
+      <c r="P6" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q6" s="0" t="str">
+        <f aca="false">O6&amp;" "&amp;P6&amp;","</f>
         <v>clasificador_fuente_financiamiento bigint,</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="R6" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O6&amp;" FOREIGN KEY ("&amp;O6&amp;") REFERENCES "&amp;IF(LEFT(O6,5)="fecha","dim_tiempo",IF(LEFT(O6,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O6))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_fuente_financiamiento FOREIGN KEY (clasificador_fuente_financiamiento) REFERENCES dim_clasificador_fuente_financiamiento(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R6" s="0" t="str">
-        <f aca="false">P6&amp;" "&amp;Q6&amp;","</f>
-        <v>fecha_firma_contrato bigint,</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>26</v>
+      <c r="T6" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
       </c>
       <c r="U6" s="0" t="str">
         <f aca="false">S6&amp;" "&amp;T6&amp;","</f>
+        <v>fecha_firma_contrato bigint,</v>
+      </c>
+      <c r="V6" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;S6&amp;" FOREIGN KEY ("&amp;S6&amp;") REFERENCES "&amp;IF(LEFT(S6,5)="fecha","dim_tiempo",IF(LEFT(S6,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;S6))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_firma_contrato FOREIGN KEY (fecha_firma_contrato) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="0" t="str">
+        <f aca="false">W6&amp;" "&amp;X6&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
     </row>
@@ -1128,83 +1186,84 @@
         <f aca="false">D7&amp;" "&amp;E7&amp;","</f>
         <v>funcion_descripcion character varying,</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="K7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="I7" s="0" t="str">
-        <f aca="false">G7&amp;" "&amp;H7&amp;","</f>
-        <v>contrato bigint,</v>
-      </c>
-      <c r="J7" s="0" t="s">
+      <c r="L7" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">K7&amp;" "&amp;L7&amp;","</f>
+        <v>clasificador_geografico bigint,</v>
+      </c>
+      <c r="N7" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K7&amp;" FOREIGN KEY ("&amp;K7&amp;") REFERENCES "&amp;IF(LEFT(K7,5)="fecha","dim_tiempo",IF(LEFT(K7,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K7))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_geografico FOREIGN KEY (clasificador_geografico) REFERENCES dim_clasificador_geografico(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q7" s="0" t="str">
+        <f aca="false">O7&amp;" "&amp;P7&amp;","</f>
+        <v>clasificador_geografico bigint,</v>
+      </c>
+      <c r="R7" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O7&amp;" FOREIGN KEY ("&amp;O7&amp;") REFERENCES "&amp;IF(LEFT(O7,5)="fecha","dim_tiempo",IF(LEFT(O7,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O7))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_geografico FOREIGN KEY (clasificador_geografico) REFERENCES dim_clasificador_geografico(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="L7" s="0" t="str">
-        <f aca="false">J7&amp;" "&amp;K7&amp;","</f>
-        <v>clasificador_geografico bigint,</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O7" s="0" t="str">
-        <f aca="false">M7&amp;" "&amp;N7&amp;","</f>
-        <v>clasificador_geografico bigint,</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R7" s="0" t="str">
-        <f aca="false">P7&amp;" "&amp;Q7&amp;","</f>
-        <v>junk_contrato bigint,</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>39</v>
+      <c r="T7" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
       </c>
       <c r="U7" s="0" t="str">
         <f aca="false">S7&amp;" "&amp;T7&amp;","</f>
+        <v>junk_contrato bigint,</v>
+      </c>
+      <c r="V7" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;S7&amp;" FOREIGN KEY ("&amp;S7&amp;") REFERENCES "&amp;IF(LEFT(S7,5)="fecha","dim_tiempo",IF(LEFT(S7,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;S7))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_junk_contrato FOREIGN KEY (junk_contrato) REFERENCES dim_junk_contrato(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="0" t="str">
+        <f aca="false">W7&amp;" "&amp;X7&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="str">
-        <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <f aca="false">Sheet2!$B$5</f>
+        <v>Numeric(7,0)</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">A8&amp;" "&amp;B8&amp;","</f>
-        <v>unidad_jerarquica_codigo numeric(5,0),</v>
+        <v>unidad_jerarquica_codigo Numeric(7,0),</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F8" s="0" t="str">
         <f aca="false">D8&amp;" "&amp;E8&amp;","</f>
-        <v>subfuncion_codigo numeric(5,0),</v>
+        <v>subfuncion_codigo Numeric(5,0),</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>12</v>
@@ -1217,53 +1276,65 @@
         <f aca="false">G8&amp;" "&amp;H8&amp;","</f>
         <v>clasificador_entidad bigint,</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G8&amp;" FOREIGN KEY ("&amp;G8&amp;") REFERENCES "&amp;IF(LEFT(G8,5)="fecha","dim_tiempo",IF(LEFT(G8,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G8))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_entidad FOREIGN KEY (clasificador_entidad) REFERENCES dim_clasificador_entidad(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">K8&amp;" "&amp;L8&amp;","</f>
+        <v>clasificador_control_financiero bigint,</v>
+      </c>
+      <c r="N8" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K8&amp;" FOREIGN KEY ("&amp;K8&amp;") REFERENCES "&amp;IF(LEFT(K8,5)="fecha","dim_tiempo",IF(LEFT(K8,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K8))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_control_financiero FOREIGN KEY (clasificador_control_financiero) REFERENCES dim_clasificador_control_financiero(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q8" s="0" t="str">
+        <f aca="false">O8&amp;" "&amp;P8&amp;","</f>
+        <v>clasificador_control_financiero bigint,</v>
+      </c>
+      <c r="R8" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O8&amp;" FOREIGN KEY ("&amp;O8&amp;") REFERENCES "&amp;IF(LEFT(O8,5)="fecha","dim_tiempo",IF(LEFT(O8,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O8))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_control_financiero FOREIGN KEY (clasificador_control_financiero) REFERENCES dim_clasificador_control_financiero(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="L8" s="0" t="str">
-        <f aca="false">J8&amp;" "&amp;K8&amp;","</f>
-        <v>clasificador_control_financiero bigint,</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O8" s="0" t="str">
-        <f aca="false">M8&amp;" "&amp;N8&amp;","</f>
-        <v>clasificador_control_financiero bigint,</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" s="0" t="str">
+      <c r="T8" s="0" t="str">
         <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
-      </c>
-      <c r="R8" s="0" t="str">
-        <f aca="false">P8&amp;" "&amp;Q8&amp;","</f>
-        <v>id_llamado numeric(13,0),</v>
-      </c>
-      <c r="S8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="T8" s="0" t="s">
-        <v>45</v>
+        <v>Numeric(7,0)</v>
       </c>
       <c r="U8" s="0" t="str">
         <f aca="false">S8&amp;" "&amp;T8&amp;","</f>
+        <v>id_llamado Numeric(7,0),</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" s="0" t="str">
+        <f aca="false">W8&amp;" "&amp;X8&amp;","</f>
         <v>checksum character varying,</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -1274,7 +1345,7 @@
         <v>unidad_jerarquica_descripcion character varying,</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -1295,55 +1366,67 @@
         <f aca="false">G9&amp;" "&amp;H9&amp;","</f>
         <v>clasificador_programa bigint,</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G9&amp;" FOREIGN KEY ("&amp;G9&amp;") REFERENCES "&amp;IF(LEFT(G9,5)="fecha","dim_tiempo",IF(LEFT(G9,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G9))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_programa FOREIGN KEY (clasificador_programa) REFERENCES dim_clasificador_programa(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">K9&amp;" "&amp;L9&amp;","</f>
+        <v>fecha_ingreso bigint,</v>
+      </c>
+      <c r="N9" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K9&amp;" FOREIGN KEY ("&amp;K9&amp;") REFERENCES "&amp;IF(LEFT(K9,5)="fecha","dim_tiempo",IF(LEFT(K9,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K9))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_ingreso FOREIGN KEY (fecha_ingreso) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="L9" s="0" t="str">
-        <f aca="false">J9&amp;" "&amp;K9&amp;","</f>
-        <v>fecha_ingreso bigint,</v>
-      </c>
-      <c r="M9" s="0" t="s">
+      <c r="P9" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q9" s="0" t="str">
+        <f aca="false">O9&amp;" "&amp;P9&amp;","</f>
+        <v>clasificador_entidad_destino bigint,</v>
+      </c>
+      <c r="R9" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O9&amp;" FOREIGN KEY ("&amp;O9&amp;") REFERENCES "&amp;IF(LEFT(O9,5)="fecha","dim_tiempo",IF(LEFT(O9,6)="cuenta","dim_cuenta_bancaria","dim_clasificador_entidad"))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_entidad_destino FOREIGN KEY (clasificador_entidad_destino) REFERENCES dim_clasificador_entidad(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S9" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="N9" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O9" s="0" t="str">
-        <f aca="false">M9&amp;" "&amp;N9&amp;","</f>
-        <v>clasificador_entidad_destino bigint,</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q9" s="0" t="str">
-        <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
-      </c>
-      <c r="R9" s="0" t="str">
-        <f aca="false">P9&amp;" "&amp;Q9&amp;","</f>
-        <v>codigo_contratacion numeric(13,0),</v>
+      <c r="T9" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
       </c>
       <c r="U9" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;S1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_categoria_dncp PRIMARY KEY (id) )</v>
+        <f aca="false">S9&amp;" "&amp;T9&amp;","</f>
+        <v>codigo_contratacion character varying,</v>
+      </c>
+      <c r="Y9" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;W1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_categoria_dncp PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">A10&amp;" "&amp;B10&amp;","</f>
-        <v>uaf_codigo numeric(5,0),</v>
+        <v>uaf_codigo Numeric(5,0),</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>25</v>
@@ -1366,50 +1449,62 @@
         <f aca="false">G10&amp;" "&amp;H10&amp;","</f>
         <v>clasificador_objeto_gasto bigint,</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G10&amp;" FOREIGN KEY ("&amp;G10&amp;") REFERENCES "&amp;IF(LEFT(G10,5)="fecha","dim_tiempo",IF(LEFT(G10,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G10))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_objeto_gasto FOREIGN KEY (clasificador_objeto_gasto) REFERENCES dim_clasificador_objeto_gasto(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L10" s="0" t="str">
-        <f aca="false">J10&amp;" "&amp;K10&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">K10&amp;" "&amp;L10&amp;","</f>
         <v>fecha_aprobacion bigint,</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="N10" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K10&amp;" FOREIGN KEY ("&amp;K10&amp;") REFERENCES "&amp;IF(LEFT(K10,5)="fecha","dim_tiempo",IF(LEFT(K10,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K10))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_aprobacion FOREIGN KEY (fecha_aprobacion) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q10" s="0" t="str">
+        <f aca="false">O10&amp;" "&amp;P10&amp;","</f>
+        <v>fecha_generacion bigint,</v>
+      </c>
+      <c r="R10" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O10&amp;" FOREIGN KEY ("&amp;O10&amp;") REFERENCES "&amp;IF(LEFT(O10,5)="fecha","dim_tiempo",IF(LEFT(O10,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O10))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_generacion FOREIGN KEY (fecha_generacion) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S10" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O10" s="0" t="str">
-        <f aca="false">M10&amp;" "&amp;N10&amp;","</f>
-        <v>fecha_generacion bigint,</v>
-      </c>
-      <c r="P10" s="0" t="s">
+      <c r="T10" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="U10" s="0" t="str">
+        <f aca="false">S10&amp;" "&amp;T10&amp;","</f>
+        <v>monto_adjudicado Numeric(17,2),</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q10" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="R10" s="0" t="str">
-        <f aca="false">P10&amp;" "&amp;Q10&amp;","</f>
-        <v>monto_adjudicado numeric(15,2),</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;S10&amp;" ("</f>
+      <c r="Y10" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;W10&amp;" ("</f>
         <v>CREATE TABLE dim_tipo_procedimiento_dncp (</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -1440,67 +1535,79 @@
         <f aca="false">G11&amp;" "&amp;H11&amp;","</f>
         <v>clasificador_fuente_financiamiento bigint,</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G11&amp;" FOREIGN KEY ("&amp;G11&amp;") REFERENCES "&amp;IF(LEFT(G11,5)="fecha","dim_tiempo",IF(LEFT(G11,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G11))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_fuente_financiamiento FOREIGN KEY (clasificador_fuente_financiamiento) REFERENCES dim_clasificador_fuente_financiamiento(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">K11&amp;" "&amp;L11&amp;","</f>
+        <v>fecha_recepcion_tesoro bigint,</v>
+      </c>
+      <c r="N11" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K11&amp;" FOREIGN KEY ("&amp;K11&amp;") REFERENCES "&amp;IF(LEFT(K11,5)="fecha","dim_tiempo",IF(LEFT(K11,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K11))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_recepcion_tesoro FOREIGN KEY (fecha_recepcion_tesoro) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O11" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="L11" s="0" t="str">
-        <f aca="false">J11&amp;" "&amp;K11&amp;","</f>
-        <v>fecha_recepcion_tesoro bigint,</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O11" s="0" t="str">
-        <f aca="false">M11&amp;" "&amp;N11&amp;","</f>
+      <c r="P11" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q11" s="0" t="str">
+        <f aca="false">O11&amp;" "&amp;P11&amp;","</f>
         <v>fecha_deposito bigint,</v>
       </c>
       <c r="R11" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;P1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_fact_contrato PRIMARY KEY (id) )</v>
-      </c>
-      <c r="S11" s="0" t="s">
+        <f aca="false">"CONSTRAINT fk_"&amp;O11&amp;" FOREIGN KEY ("&amp;O11&amp;") REFERENCES "&amp;IF(LEFT(O11,5)="fecha","dim_tiempo",IF(LEFT(O11,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O11))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_fecha_deposito FOREIGN KEY (fecha_deposito) REFERENCES dim_tiempo(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="U11" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;S1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_fact_contrato PRIMARY KEY (id) );</v>
+      </c>
+      <c r="W11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="X11" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="U11" s="0" t="str">
-        <f aca="false">S11&amp;" "&amp;T11&amp;","</f>
+      <c r="Y11" s="0" t="str">
+        <f aca="false">W11&amp;" "&amp;X11&amp;","</f>
         <v>id bigserial,</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">A12&amp;" "&amp;B12&amp;","</f>
-        <v>unidad_responsable_codigo numeric(5,0),</v>
+        <v>unidad_responsable_codigo Numeric(5,0),</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F12" s="0" t="str">
         <f aca="false">D12&amp;" "&amp;E12&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">Sheet2!$B$4</f>
@@ -1510,51 +1617,64 @@
         <f aca="false">G12&amp;" "&amp;H12&amp;","</f>
         <v>clasificador_geografico bigint,</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G12&amp;" FOREIGN KEY ("&amp;G12&amp;") REFERENCES "&amp;IF(LEFT(G12,5)="fecha","dim_tiempo",IF(LEFT(G12,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G12))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_geografico FOREIGN KEY (clasificador_geografico) REFERENCES dim_clasificador_geografico(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
       <c r="L12" s="0" t="str">
-        <f aca="false">J12&amp;" "&amp;K12&amp;","</f>
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <f aca="false">K12&amp;" "&amp;L12&amp;","</f>
         <v>proveedor bigint,</v>
       </c>
-      <c r="M12" s="0" t="s">
+      <c r="N12" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K12&amp;" FOREIGN KEY ("&amp;K12&amp;") REFERENCES "&amp;IF(LEFT(K12,5)="fecha","dim_tiempo",IF(LEFT(K12,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K12))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_proveedor FOREIGN KEY (proveedor) REFERENCES dim_proveedor(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O12" s="0" t="str">
-        <f aca="false">M12&amp;" "&amp;N12&amp;","</f>
+      <c r="P12" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q12" s="0" t="str">
+        <f aca="false">O12&amp;" "&amp;P12&amp;","</f>
         <v>proveedor bigint,</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O12&amp;" FOREIGN KEY ("&amp;O12&amp;") REFERENCES "&amp;IF(LEFT(O12,5)="fecha","dim_tiempo",IF(LEFT(O12,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O12))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_proveedor FOREIGN KEY (proveedor) REFERENCES dim_proveedor(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;S12&amp;" ("</f>
+        <v>CREATE TABLE dim_junk_contrato (</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;P12&amp;" ("</f>
-        <v>CREATE TABLE dim_junk_contrato (</v>
-      </c>
-      <c r="S12" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="T12" s="0" t="str">
+      <c r="X12" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
-      </c>
-      <c r="U12" s="0" t="str">
-        <f aca="false">S12&amp;" "&amp;T12&amp;","</f>
-        <v>tipo_procedimiento_codigo numeric(5,0),</v>
+        <v>Numeric(5,0)</v>
+      </c>
+      <c r="Y12" s="0" t="str">
+        <f aca="false">W12&amp;" "&amp;X12&amp;","</f>
+        <v>tipo_procedimiento_codigo Numeric(5,0),</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -1565,17 +1685,17 @@
         <v>unidad_responsable_descripcion character varying,</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="F13" s="0" t="str">
         <f aca="false">D13&amp;" "&amp;E13&amp;","</f>
         <v>checksum character varying,</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">Sheet2!$B$4</f>
@@ -1585,47 +1705,59 @@
         <f aca="false">G13&amp;" "&amp;H13&amp;","</f>
         <v>clasificador_control_financiero bigint,</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G13&amp;" FOREIGN KEY ("&amp;G13&amp;") REFERENCES "&amp;IF(LEFT(G13,5)="fecha","dim_tiempo",IF(LEFT(G13,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G13))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_clasificador_control_financiero FOREIGN KEY (clasificador_control_financiero) REFERENCES dim_clasificador_control_financiero(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M13" s="0" t="str">
+        <f aca="false">K13&amp;" "&amp;L13&amp;","</f>
+        <v>junk_str bigint,</v>
+      </c>
+      <c r="N13" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K13&amp;" FOREIGN KEY ("&amp;K13&amp;") REFERENCES "&amp;IF(LEFT(K13,5)="fecha","dim_tiempo",IF(LEFT(K13,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K13))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_junk_str FOREIGN KEY (junk_str) REFERENCES dim_junk_str(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O13" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="L13" s="0" t="str">
-        <f aca="false">J13&amp;" "&amp;K13&amp;","</f>
-        <v>junk_str bigint,</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O13" s="0" t="str">
-        <f aca="false">M13&amp;" "&amp;N13&amp;","</f>
+      <c r="P13" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q13" s="0" t="str">
+        <f aca="false">O13&amp;" "&amp;P13&amp;","</f>
         <v>cuenta_origen bigint,</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="R13" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O13&amp;" FOREIGN KEY ("&amp;O13&amp;") REFERENCES "&amp;IF(LEFT(O13,5)="fecha","dim_tiempo",IF(LEFT(O13,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O13))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_cuenta_origen FOREIGN KEY (cuenta_origen) REFERENCES dim_cuenta_bancaria(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S13" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="T13" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="R13" s="0" t="str">
-        <f aca="false">P13&amp;" "&amp;Q13&amp;","</f>
-        <v>id bigserial,</v>
-      </c>
-      <c r="S13" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="T13" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
       </c>
       <c r="U13" s="0" t="str">
         <f aca="false">S13&amp;" "&amp;T13&amp;","</f>
+        <v>id bigserial,</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="X13" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="Y13" s="0" t="str">
+        <f aca="false">W13&amp;" "&amp;X13&amp;","</f>
         <v>tipo_procedimiento_descripcion character varying,</v>
       </c>
     </row>
@@ -1641,11 +1773,11 @@
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
       <c r="F14" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;D1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_funcion PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;D1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_funcion PRIMARY KEY (id) );</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H14" s="0" t="str">
         <f aca="false">Sheet2!$B$4</f>
@@ -1655,47 +1787,59 @@
         <f aca="false">G14&amp;" "&amp;H14&amp;","</f>
         <v>junk_obligacion bigint,</v>
       </c>
-      <c r="J14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="0" t="str">
-        <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
+      <c r="J14" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;G14&amp;" FOREIGN KEY ("&amp;G14&amp;") REFERENCES "&amp;IF(LEFT(G14,5)="fecha","dim_tiempo",IF(LEFT(G14,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;G14))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_junk_obligacion FOREIGN KEY (junk_obligacion) REFERENCES dim_junk_obligacion(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="L14" s="0" t="str">
-        <f aca="false">J14&amp;" "&amp;K14&amp;","</f>
-        <v>cuenta_origen numeric(13,0),</v>
-      </c>
-      <c r="M14" s="0" t="s">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">K14&amp;" "&amp;L14&amp;","</f>
+        <v>cuenta_origen bigint,</v>
+      </c>
+      <c r="N14" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;K14&amp;" FOREIGN KEY ("&amp;K14&amp;") REFERENCES "&amp;IF(LEFT(K14,5)="fecha","dim_tiempo",IF(LEFT(K14,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;K14))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_cuenta_origen FOREIGN KEY (cuenta_origen) REFERENCES dim_cuenta_bancaria(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q14" s="0" t="str">
+        <f aca="false">O14&amp;" "&amp;P14&amp;","</f>
+        <v>cuenta_destino bigint,</v>
+      </c>
+      <c r="R14" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O14&amp;" FOREIGN KEY ("&amp;O14&amp;") REFERENCES "&amp;IF(LEFT(O14,5)="fecha","dim_tiempo",IF(LEFT(O14,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O14))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_cuenta_destino FOREIGN KEY (cuenta_destino) REFERENCES dim_cuenta_bancaria(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O14" s="0" t="str">
-        <f aca="false">M14&amp;" "&amp;N14&amp;","</f>
-        <v>cuenta_destino bigint,</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R14" s="0" t="str">
-        <f aca="false">P14&amp;" "&amp;Q14&amp;","</f>
-        <v>nombre_licitacion character varying,</v>
-      </c>
-      <c r="S14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="T14" s="0" t="s">
-        <v>26</v>
+      <c r="T14" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
       </c>
       <c r="U14" s="0" t="str">
         <f aca="false">S14&amp;" "&amp;T14&amp;","</f>
+        <v>nombre_licitacion character varying,</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y14" s="0" t="str">
+        <f aca="false">W14&amp;" "&amp;X14&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
     </row>
@@ -1711,7 +1855,7 @@
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="str">
@@ -1719,66 +1863,70 @@
         <v>CREATE TABLE dim_clasificador_fuente_financiamiento (</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
+        <v>Numeric(7,0)</v>
       </c>
       <c r="I15" s="0" t="str">
         <f aca="false">G15&amp;" "&amp;H15&amp;","</f>
-        <v>numero_obligacion numeric(13,0),</v>
-      </c>
-      <c r="J15" s="0" t="s">
+        <v>numero_obligacion Numeric(7,0),</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">Sheet2!$B$5</f>
+        <v>Numeric(7,0)</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">K15&amp;" "&amp;L15&amp;","</f>
+        <v>numero_str Numeric(7,0),</v>
+      </c>
+      <c r="O15" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="0" t="str">
-        <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
-      </c>
-      <c r="L15" s="0" t="str">
-        <f aca="false">J15&amp;" "&amp;K15&amp;","</f>
-        <v>numero_str numeric(13,0),</v>
-      </c>
-      <c r="M15" s="0" t="s">
+      <c r="P15" s="0" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="Q15" s="0" t="str">
+        <f aca="false">O15&amp;" "&amp;P15&amp;","</f>
+        <v>junk_ot bigint,</v>
+      </c>
+      <c r="R15" s="0" t="str">
+        <f aca="false">"CONSTRAINT fk_"&amp;O15&amp;" FOREIGN KEY ("&amp;O15&amp;") REFERENCES "&amp;IF(LEFT(O15,5)="fecha","dim_tiempo",IF(LEFT(O15,6)="cuenta","dim_cuenta_bancaria","dim_"&amp;O15))&amp;"(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,"</f>
+        <v>CONSTRAINT fk_junk_ot FOREIGN KEY (junk_ot) REFERENCES dim_junk_ot(id) MATCH SIMPLE ON UPDATE NO ACTION ON DELETE NO ACTION,</v>
+      </c>
+      <c r="S15" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="N15" s="0" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="O15" s="0" t="str">
-        <f aca="false">M15&amp;" "&amp;N15&amp;","</f>
-        <v>junk_ot bigint,</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q15" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R15" s="0" t="str">
-        <f aca="false">P15&amp;" "&amp;Q15&amp;","</f>
-        <v>convocante character varying,</v>
-      </c>
-      <c r="S15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="T15" s="0" t="s">
-        <v>26</v>
+      <c r="T15" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
       </c>
       <c r="U15" s="0" t="str">
         <f aca="false">S15&amp;" "&amp;T15&amp;","</f>
+        <v>convocante character varying,</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y15" s="0" t="str">
+        <f aca="false">W15&amp;" "&amp;X15&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">A16&amp;" "&amp;B16&amp;","</f>
@@ -1795,66 +1943,66 @@
         <v>id bigserial,</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
+        <v>Numeric(7,0)</v>
       </c>
       <c r="I16" s="0" t="str">
         <f aca="false">G16&amp;" "&amp;H16&amp;","</f>
-        <v>numero_str numeric(13,0),</v>
-      </c>
-      <c r="J16" s="0" t="s">
+        <v>numero_str Numeric(7,0),</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">K16&amp;" "&amp;L16&amp;","</f>
+        <v>monto_solicitado Numeric(17,2),</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="L16" s="0" t="str">
-        <f aca="false">J16&amp;" "&amp;K16&amp;","</f>
-        <v>monto_solicitado numeric(15,2),</v>
-      </c>
-      <c r="M16" s="0" t="s">
+      <c r="P16" s="0" t="str">
+        <f aca="false">Sheet2!$B$5</f>
+        <v>Numeric(7,0)</v>
+      </c>
+      <c r="Q16" s="0" t="str">
+        <f aca="false">O16&amp;" "&amp;P16&amp;","</f>
+        <v>numero_ot Numeric(7,0),</v>
+      </c>
+      <c r="S16" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="N16" s="0" t="str">
-        <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
-      </c>
-      <c r="O16" s="0" t="str">
-        <f aca="false">M16&amp;" "&amp;N16&amp;","</f>
-        <v>numero_ot numeric(13,0),</v>
-      </c>
-      <c r="P16" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q16" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R16" s="0" t="str">
-        <f aca="false">P16&amp;" "&amp;Q16&amp;","</f>
-        <v>estado character varying,</v>
-      </c>
-      <c r="S16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T16" s="0" t="s">
-        <v>39</v>
+      <c r="T16" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
       </c>
       <c r="U16" s="0" t="str">
         <f aca="false">S16&amp;" "&amp;T16&amp;","</f>
+        <v>estado character varying,</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y16" s="0" t="str">
+        <f aca="false">W16&amp;" "&amp;X16&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">A17&amp;" "&amp;B17&amp;","</f>
@@ -1871,129 +2019,129 @@
         <v>anho numeric(4,0),</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I17" s="0" t="str">
         <f aca="false">G17&amp;" "&amp;H17&amp;","</f>
-        <v>monto_obligado numeric(15,2),</v>
-      </c>
-      <c r="J17" s="0" t="s">
+        <v>monto_obligado Numeric(17,2),</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L17" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="M17" s="0" t="str">
+        <f aca="false">K17&amp;" "&amp;L17&amp;","</f>
+        <v>monto_deducciones Numeric(17,2),</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" s="0" t="str">
+        <f aca="false">Sheet2!$B$5</f>
+        <v>Numeric(7,0)</v>
+      </c>
+      <c r="Q17" s="0" t="str">
+        <f aca="false">O17&amp;" "&amp;P17&amp;","</f>
+        <v>numero_str Numeric(7,0),</v>
+      </c>
+      <c r="S17" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="K17" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="L17" s="0" t="str">
-        <f aca="false">J17&amp;" "&amp;K17&amp;","</f>
-        <v>monto_deducciones numeric(15,2),</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="N17" s="0" t="str">
-        <f aca="false">Sheet2!$B$5</f>
-        <v>numeric(13,0)</v>
-      </c>
-      <c r="O17" s="0" t="str">
-        <f aca="false">M17&amp;" "&amp;N17&amp;","</f>
-        <v>numero_str numeric(13,0),</v>
-      </c>
-      <c r="P17" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q17" s="0" t="str">
+      <c r="T17" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
-      </c>
-      <c r="R17" s="0" t="str">
-        <f aca="false">P17&amp;" "&amp;Q17&amp;","</f>
-        <v>moneda_codigo numeric(5,0),</v>
-      </c>
-      <c r="S17" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="T17" s="0" t="s">
-        <v>45</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="U17" s="0" t="str">
         <f aca="false">S17&amp;" "&amp;T17&amp;","</f>
+        <v>moneda_codigo Numeric(5,0),</v>
+      </c>
+      <c r="W17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y17" s="0" t="str">
+        <f aca="false">W17&amp;" "&amp;X17&amp;","</f>
         <v>checksum character varying,</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;A1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_entidades PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;A1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_entidad PRIMARY KEY (id) );</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F18" s="0" t="str">
         <f aca="false">D18&amp;" "&amp;E18&amp;","</f>
-        <v>fuente_financiamiento_codigo numeric(5,0),</v>
+        <v>fuente_financiamiento_codigo Numeric(5,0),</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I18" s="0" t="str">
         <f aca="false">G18&amp;" "&amp;H18&amp;","</f>
-        <v>monto_deduccion_iva numeric(15,2),</v>
-      </c>
-      <c r="L18" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;J1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_fact_str PRIMARY KEY (id) )</v>
-      </c>
-      <c r="M18" s="0" t="s">
+        <v>monto_deduccion_iva Numeric(17,2),</v>
+      </c>
+      <c r="M18" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;K1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_fact_str PRIMARY KEY (id) );</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="P18" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="Q18" s="0" t="str">
+        <f aca="false">O18&amp;" "&amp;P18&amp;","</f>
+        <v>cotizacion Numeric(17,2),</v>
+      </c>
+      <c r="S18" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="N18" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="O18" s="0" t="str">
-        <f aca="false">M18&amp;" "&amp;N18&amp;","</f>
-        <v>cotizacion numeric(15,2),</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q18" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R18" s="0" t="str">
-        <f aca="false">P18&amp;" "&amp;Q18&amp;","</f>
+      <c r="T18" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="U18" s="0" t="str">
+        <f aca="false">S18&amp;" "&amp;T18&amp;","</f>
         <v>moneda_simbolo character varying,</v>
       </c>
-      <c r="U18" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;S10&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_tipo_procedimiento_dncp PRIMARY KEY (id) )</v>
+      <c r="Y18" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;W10&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_tipo_procedimiento_dncp PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="str">
         <f aca="false">"CREATE TABLE "&amp;A19&amp;" ("</f>
         <v>CREATE TABLE dim_clasificador_programa (</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>84</v>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2004,44 +2152,45 @@
         <v>fuente_financiamiento_descripcion character varying,</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H19" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I19" s="0" t="str">
         <f aca="false">G19&amp;" "&amp;H19&amp;","</f>
-        <v>monto_deduccion_renta numeric(15,2),</v>
-      </c>
-      <c r="J19" s="1" t="s">
+        <v>monto_deduccion_renta Numeric(17,2),</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;K19&amp;" ("</f>
+        <v>CREATE TABLE dim_junk_str (</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;J19&amp;" ("</f>
-        <v>CREATE TABLE dim_junk_str (</v>
-      </c>
-      <c r="M19" s="0" t="s">
+      <c r="P19" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="Q19" s="0" t="str">
+        <f aca="false">O19&amp;" "&amp;P19&amp;","</f>
+        <v>monto_ot Numeric(17,2),</v>
+      </c>
+      <c r="S19" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="N19" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="O19" s="0" t="str">
-        <f aca="false">M19&amp;" "&amp;N19&amp;","</f>
-        <v>monto_ot numeric(15,2),</v>
-      </c>
-      <c r="P19" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q19" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R19" s="0" t="str">
-        <f aca="false">P19&amp;" "&amp;Q19&amp;","</f>
+      <c r="T19" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="U19" s="0" t="str">
+        <f aca="false">S19&amp;" "&amp;T19&amp;","</f>
         <v>moneda_descripcion character varying,</v>
       </c>
     </row>
@@ -2057,57 +2206,57 @@
         <v>id bigserial,</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F20" s="0" t="str">
         <f aca="false">D20&amp;" "&amp;E20&amp;","</f>
-        <v>organismo_financiador_codigo numeric(5,0),</v>
+        <v>organismo_financiador_codigo Numeric(5,0),</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I20" s="0" t="str">
         <f aca="false">G20&amp;" "&amp;H20&amp;","</f>
-        <v>monto_deduccion_dncp numeric(15,2),</v>
-      </c>
-      <c r="J20" s="0" t="s">
+        <v>monto_deduccion_dncp Numeric(17,2),</v>
+      </c>
+      <c r="K20" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="L20" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="0" t="str">
-        <f aca="false">J20&amp;" "&amp;K20&amp;","</f>
+      <c r="M20" s="0" t="str">
+        <f aca="false">K20&amp;" "&amp;L20&amp;","</f>
         <v>id bigserial,</v>
       </c>
-      <c r="M20" s="0" t="s">
+      <c r="O20" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P20" s="0" t="str">
+        <f aca="false">Sheet2!$B$2</f>
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="Q20" s="0" t="str">
+        <f aca="false">O20&amp;" "&amp;P20&amp;","</f>
+        <v>monto_ot_gs Numeric(17,2),</v>
+      </c>
+      <c r="S20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="N20" s="0" t="str">
-        <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="O20" s="0" t="str">
-        <f aca="false">M20&amp;" "&amp;N20&amp;","</f>
-        <v>monto_ot_gs numeric(15,2),</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q20" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="R20" s="0" t="str">
-        <f aca="false">P20&amp;" "&amp;Q20&amp;","</f>
+      <c r="T20" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="U20" s="0" t="str">
+        <f aca="false">S20&amp;" "&amp;T20&amp;","</f>
         <v>vigencia_contrato character varying,</v>
       </c>
     </row>
@@ -2123,7 +2272,7 @@
         <v>anho numeric(4,0),</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2134,60 +2283,60 @@
         <v>organismo_financiador_descripcion character varying,</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I21" s="0" t="str">
         <f aca="false">G21&amp;" "&amp;H21&amp;","</f>
-        <v>monto_deduccion_incumplimiento_contrato numeric(15,2),</v>
-      </c>
-      <c r="J21" s="0" t="s">
+        <v>monto_deduccion_incumplimiento_contrato Numeric(17,2),</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="L21" s="0" t="str">
+        <f aca="false">Sheet2!$B$1</f>
+        <v>Numeric(5,0)</v>
+      </c>
+      <c r="M21" s="0" t="str">
+        <f aca="false">K21&amp;" "&amp;L21&amp;","</f>
+        <v>situacion_str_codigo Numeric(5,0),</v>
+      </c>
+      <c r="O21" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="K21" s="0" t="str">
-        <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
-      </c>
-      <c r="L21" s="0" t="str">
-        <f aca="false">J21&amp;" "&amp;K21&amp;","</f>
-        <v>situacion_str_codigo numeric(5,0),</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="N21" s="0" t="str">
+      <c r="P21" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
-      </c>
-      <c r="O21" s="0" t="str">
-        <f aca="false">M21&amp;" "&amp;N21&amp;","</f>
-        <v>monto_ot_destino numeric(15,2),</v>
-      </c>
-      <c r="P21" s="0" t="s">
+        <v>Numeric(17,2)</v>
+      </c>
+      <c r="Q21" s="0" t="str">
+        <f aca="false">O21&amp;" "&amp;P21&amp;","</f>
+        <v>monto_ot_destino Numeric(17,2),</v>
+      </c>
+      <c r="S21" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="T21" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="R21" s="0" t="str">
-        <f aca="false">P21&amp;" "&amp;Q21&amp;","</f>
+      <c r="U21" s="0" t="str">
+        <f aca="false">S21&amp;" "&amp;T21&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">A22&amp;" "&amp;B22&amp;","</f>
-        <v>tipo_presupuesto_codigo numeric(5,0),</v>
+        <v>tipo_presupuesto_codigo Numeric(5,0),</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>25</v>
@@ -2200,45 +2349,45 @@
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">Sheet2!$B$2</f>
-        <v>numeric(15,2)</v>
+        <v>Numeric(17,2)</v>
       </c>
       <c r="I22" s="0" t="str">
         <f aca="false">G22&amp;" "&amp;H22&amp;","</f>
-        <v>monto_deduccion_otras numeric(15,2),</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
+        <v>monto_deduccion_otras Numeric(17,2),</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="L22" s="0" t="str">
-        <f aca="false">J22&amp;" "&amp;K22&amp;","</f>
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="M22" s="0" t="str">
+        <f aca="false">K22&amp;" "&amp;L22&amp;","</f>
         <v>situacion_str_descripcion character varying,</v>
       </c>
-      <c r="O22" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;M1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_fact_ot PRIMARY KEY (id) )</v>
-      </c>
-      <c r="P22" s="0" t="s">
+      <c r="Q22" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;O1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_fact_ot PRIMARY KEY (id) );</v>
+      </c>
+      <c r="S22" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="T22" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="R22" s="0" t="str">
-        <f aca="false">P22&amp;" "&amp;Q22&amp;","</f>
+      <c r="U22" s="0" t="str">
+        <f aca="false">S22&amp;" "&amp;T22&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2259,104 +2408,106 @@
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
       <c r="I23" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;G1&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_fact_obligacion PRIMARY KEY (id) )</v>
-      </c>
-      <c r="J23" s="0" t="s">
+        <f aca="false">"CONSTRAINT pk_"&amp;G1&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_fact_obligacion PRIMARY KEY (id) );</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="0" t="str">
+        <f aca="false">Sheet2!$B$1</f>
+        <v>Numeric(5,0)</v>
+      </c>
+      <c r="M23" s="0" t="str">
+        <f aca="false">K23&amp;" "&amp;L23&amp;","</f>
+        <v>tipo_str_codigo Numeric(5,0),</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K23" s="0" t="str">
-        <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
-      </c>
-      <c r="L23" s="0" t="str">
-        <f aca="false">J23&amp;" "&amp;K23&amp;","</f>
-        <v>tipo_str_codigo numeric(5,0),</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N23" s="1"/>
-      <c r="O23" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;M23&amp;" ("</f>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;O23&amp;" ("</f>
         <v>CREATE TABLE dim_junk_ot (</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="R23" s="2"/>
+      <c r="S23" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T23" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="Q23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="R23" s="0" t="str">
-        <f aca="false">P23&amp;" "&amp;Q23&amp;","</f>
+      <c r="U23" s="0" t="str">
+        <f aca="false">S23&amp;" "&amp;T23&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">A24&amp;" "&amp;B24&amp;","</f>
-        <v>programa_codigo numeric(5,0),</v>
+        <v>programa_codigo Numeric(5,0),</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F24" s="0" t="str">
         <f aca="false">D24&amp;" "&amp;E24&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="2" t="str">
         <f aca="false">"CREATE TABLE "&amp;G24&amp;" ("</f>
         <v>CREATE TABLE dim_junk_obligacion (</v>
       </c>
-      <c r="J24" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="K24" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
+      <c r="J24" s="2"/>
+      <c r="K24" s="0" t="s">
+        <v>104</v>
       </c>
       <c r="L24" s="0" t="str">
-        <f aca="false">J24&amp;" "&amp;K24&amp;","</f>
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="M24" s="0" t="str">
+        <f aca="false">K24&amp;" "&amp;L24&amp;","</f>
         <v>tipo_str_descripcion character varying,</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="O24" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="P24" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="O24" s="0" t="str">
-        <f aca="false">M24&amp;" "&amp;N24&amp;","</f>
+      <c r="Q24" s="0" t="str">
+        <f aca="false">O24&amp;" "&amp;P24&amp;","</f>
         <v>id bigserial,</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="S24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="T24" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="Q24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="R24" s="0" t="str">
-        <f aca="false">P24&amp;" "&amp;Q24&amp;","</f>
+      <c r="U24" s="0" t="str">
+        <f aca="false">S24&amp;" "&amp;T24&amp;","</f>
         <v>checksum character varying,</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2367,10 +2518,10 @@
         <v>programa_descripcion character varying,</v>
       </c>
       <c r="D25" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="F25" s="0" t="str">
         <f aca="false">D25&amp;" "&amp;E25&amp;","</f>
@@ -2386,94 +2537,95 @@
         <f aca="false">G25&amp;" "&amp;H25&amp;","</f>
         <v>id bigserial,</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="K25" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="M25" s="0" t="str">
+        <f aca="false">K25&amp;" "&amp;L25&amp;","</f>
+        <v>descripcion_str character varying,</v>
+      </c>
+      <c r="O25" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="L25" s="0" t="str">
-        <f aca="false">J25&amp;" "&amp;K25&amp;","</f>
-        <v>descripcion_str character varying,</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="N25" s="0" t="str">
+      <c r="P25" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
-      </c>
-      <c r="O25" s="0" t="str">
-        <f aca="false">M25&amp;" "&amp;N25&amp;","</f>
-        <v>concepto_codigo numeric(5,0),</v>
-      </c>
-      <c r="R25" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;P12&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_junk_contrato PRIMARY KEY (id) )</v>
+        <v>Numeric(5,0)</v>
+      </c>
+      <c r="Q25" s="0" t="str">
+        <f aca="false">O25&amp;" "&amp;P25&amp;","</f>
+        <v>concepto_codigo Numeric(5,0),</v>
+      </c>
+      <c r="U25" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;S12&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_junk_contrato PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">A26&amp;" "&amp;B26&amp;","</f>
-        <v>subprograma_codigo numeric(5,0),</v>
+        <v>subprograma_codigo Numeric(5,0),</v>
       </c>
       <c r="F26" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;D15&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_fuente_financiamiento PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;D15&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_fuente_financiamiento PRIMARY KEY (id) );</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H26" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="I26" s="0" t="str">
         <f aca="false">G26&amp;" "&amp;H26&amp;","</f>
-        <v>concepto_obligacion_codigo numeric(5,0),</v>
-      </c>
-      <c r="J26" s="0" t="s">
+        <v>concepto_obligacion_codigo Numeric(5,0),</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="L26" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="M26" s="0" t="str">
+        <f aca="false">K26&amp;" "&amp;L26&amp;","</f>
+        <v>detalle_str character varying,</v>
+      </c>
+      <c r="O26" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="K26" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="L26" s="0" t="str">
-        <f aca="false">J26&amp;" "&amp;K26&amp;","</f>
-        <v>detalle_str character varying,</v>
-      </c>
-      <c r="M26" s="0" t="s">
+      <c r="P26" s="0" t="str">
+        <f aca="false">Sheet2!$B$3</f>
+        <v>character varying</v>
+      </c>
+      <c r="Q26" s="0" t="str">
+        <f aca="false">O26&amp;" "&amp;P26&amp;","</f>
+        <v>concepto_descripcion character varying,</v>
+      </c>
+      <c r="S26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N26" s="0" t="str">
-        <f aca="false">Sheet2!$B$3</f>
-        <v>character varying</v>
-      </c>
-      <c r="O26" s="0" t="str">
-        <f aca="false">M26&amp;" "&amp;N26&amp;","</f>
-        <v>concepto_descripcion character varying,</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="2" t="str">
-        <f aca="false">"CREATE TABLE "&amp;P26&amp;" ("</f>
+      <c r="T26" s="3"/>
+      <c r="U26" s="2" t="str">
+        <f aca="false">"CREATE TABLE "&amp;S26&amp;" ("</f>
         <v>CREATE TABLE br_obligacion_contrato (</v>
       </c>
+      <c r="V26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2484,7 +2636,7 @@
         <v>subprograma_descripcion character varying,</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="str">
@@ -2492,7 +2644,7 @@
         <v>CREATE TABLE dim_clasificador_geografico (</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H27" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2502,48 +2654,48 @@
         <f aca="false">G27&amp;" "&amp;H27&amp;","</f>
         <v>concepto_obligacion_descripcion character varying,</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="K27" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="L27" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="0" t="str">
-        <f aca="false">J27&amp;" "&amp;K27&amp;","</f>
+      <c r="M27" s="0" t="str">
+        <f aca="false">K27&amp;" "&amp;L27&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="O27" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="P27" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O27" s="0" t="str">
-        <f aca="false">M27&amp;" "&amp;N27&amp;","</f>
+      <c r="Q27" s="0" t="str">
+        <f aca="false">O27&amp;" "&amp;P27&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
-      <c r="P27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q27" s="3" t="s">
+      <c r="T27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R27" s="0" t="str">
-        <f aca="false">P27&amp;" "&amp;Q27&amp;","</f>
+      <c r="U27" s="0" t="str">
+        <f aca="false">S27&amp;" "&amp;T27&amp;","</f>
         <v>id bigserial,</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">A28&amp;" "&amp;B28&amp;","</f>
-        <v>proyecto_codigo numeric(5,0),</v>
+        <v>proyecto_codigo Numeric(5,0),</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
@@ -2565,41 +2717,41 @@
         <f aca="false">G28&amp;" "&amp;H28&amp;","</f>
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="K28" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="L28" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="0" t="str">
-        <f aca="false">J28&amp;" "&amp;K28&amp;","</f>
+      <c r="M28" s="0" t="str">
+        <f aca="false">K28&amp;" "&amp;L28&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="O28" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="P28" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O28" s="0" t="str">
-        <f aca="false">M28&amp;" "&amp;N28&amp;","</f>
+      <c r="Q28" s="0" t="str">
+        <f aca="false">O28&amp;" "&amp;P28&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
-      <c r="P28" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q28" s="4" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R28" s="0" t="str">
-        <f aca="false">P28&amp;" "&amp;Q28&amp;","</f>
+      <c r="S28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="T28" s="4" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="U28" s="0" t="str">
+        <f aca="false">S28&amp;" "&amp;T28&amp;","</f>
         <v>obligacion bigint,</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -2610,15 +2762,15 @@
         <v>proyecto_descripcion character varying,</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E29" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F29" s="0" t="str">
         <f aca="false">D29&amp;" "&amp;E29&amp;","</f>
-        <v>pais_codigo numeric(5,0),</v>
+        <v>pais_codigo Numeric(5,0),</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>32</v>
@@ -2630,35 +2782,35 @@
         <f aca="false">G29&amp;" "&amp;H29&amp;","</f>
         <v>fecha_fin_vigencia timestamp without time zone,</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="K29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="0" t="str">
-        <f aca="false">J29&amp;" "&amp;K29&amp;","</f>
+      <c r="M29" s="0" t="str">
+        <f aca="false">K29&amp;" "&amp;L29&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
-      <c r="M29" s="0" t="s">
+      <c r="O29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="P29" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="N29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O29" s="0" t="str">
-        <f aca="false">M29&amp;" "&amp;N29&amp;","</f>
+      <c r="Q29" s="0" t="str">
+        <f aca="false">O29&amp;" "&amp;P29&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
-      <c r="P29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q29" s="4" t="str">
-        <f aca="false">Sheet2!$B$4</f>
-        <v>bigint</v>
-      </c>
-      <c r="R29" s="0" t="str">
-        <f aca="false">P29&amp;" "&amp;Q29&amp;","</f>
+      <c r="S29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="T29" s="4" t="str">
+        <f aca="false">Sheet2!$B$4</f>
+        <v>bigint</v>
+      </c>
+      <c r="U29" s="0" t="str">
+        <f aca="false">S29&amp;" "&amp;T29&amp;","</f>
         <v>contrato bigint,</v>
       </c>
     </row>
@@ -2685,38 +2837,38 @@
         <v>pais_simbolo character varying,</v>
       </c>
       <c r="G30" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="I30" s="0" t="str">
         <f aca="false">G30&amp;" "&amp;H30&amp;","</f>
         <v>actual numeric(1,0),</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="K30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="L30" s="0" t="str">
-        <f aca="false">J30&amp;" "&amp;K30&amp;","</f>
+      <c r="M30" s="0" t="str">
+        <f aca="false">K30&amp;" "&amp;L30&amp;","</f>
         <v>checksum character varying,</v>
       </c>
-      <c r="M30" s="0" t="s">
+      <c r="O30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="P30" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="N30" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="O30" s="0" t="str">
-        <f aca="false">M30&amp;" "&amp;N30&amp;","</f>
+      <c r="Q30" s="0" t="str">
+        <f aca="false">O30&amp;" "&amp;P30&amp;","</f>
         <v>checksum character varying,</v>
       </c>
-      <c r="R30" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;P26&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_br_obligacion_contrato PRIMARY KEY (id) )</v>
+      <c r="U30" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;S26&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_br_obligacion_contrato PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,30 +2894,30 @@
         <v>pais_descripcion character varying,</v>
       </c>
       <c r="G31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="I31" s="0" t="str">
         <f aca="false">G31&amp;" "&amp;H31&amp;","</f>
         <v>checksum character varying,</v>
       </c>
-      <c r="L31" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;J19&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_junk_str PRIMARY KEY (id) )</v>
-      </c>
-      <c r="O31" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;M23&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_junk_ot PRIMARY KEY (id) )</v>
+      <c r="M31" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;K19&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_junk_str PRIMARY KEY (id) );</v>
+      </c>
+      <c r="Q31" s="0" t="str">
+        <f aca="false">"CONSTRAINT pk_"&amp;O23&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_junk_ot PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">A32&amp;" "&amp;B32&amp;","</f>
@@ -2776,23 +2928,23 @@
       </c>
       <c r="E32" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F32" s="0" t="str">
         <f aca="false">D32&amp;" "&amp;E32&amp;","</f>
-        <v>departamento_codigo numeric(5,0),</v>
+        <v>departamento_codigo Numeric(5,0),</v>
       </c>
       <c r="I32" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;G24&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_junk_obligacion PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;G24&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_junk_obligacion PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">A33&amp;" "&amp;B33&amp;","</f>
@@ -2812,8 +2964,8 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;A19&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_programa PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;A19&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_programa PRIMARY KEY (id) );</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>125</v>
@@ -2881,10 +3033,10 @@
         <v>anho numeric(4,0),</v>
       </c>
       <c r="D37" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F37" s="0" t="str">
         <f aca="false">D37&amp;" "&amp;E37&amp;","</f>
@@ -2897,17 +3049,17 @@
       </c>
       <c r="B38" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">A38&amp;" "&amp;B38&amp;","</f>
-        <v>grupo_codigo numeric(5,0),</v>
+        <v>grupo_codigo Numeric(5,0),</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="F38" s="0" t="str">
         <f aca="false">D38&amp;" "&amp;E38&amp;","</f>
@@ -2927,8 +3079,8 @@
         <v>grupo_descripcion character varying,</v>
       </c>
       <c r="F39" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;D27&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_geografico PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;D27&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_geografico PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,11 +3089,11 @@
       </c>
       <c r="B40" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">A40&amp;" "&amp;B40&amp;","</f>
-        <v>subgrupo_codigo numeric(5,0),</v>
+        <v>subgrupo_codigo Numeric(5,0),</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>130</v>
@@ -2953,7 +3105,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B41" s="0" t="str">
@@ -2981,22 +3133,22 @@
       </c>
       <c r="B42" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">A42&amp;" "&amp;B42&amp;","</f>
-        <v>objeto_gasto_codigo numeric(5,0),</v>
+        <v>objeto_gasto_codigo Numeric(5,0),</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>133</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="F42" s="0" t="str">
         <f aca="false">D42&amp;" "&amp;E42&amp;","</f>
-        <v>proveedor_id numeric(5,0),</v>
+        <v>proveedor_id Numeric(5,0),</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,10 +3223,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">A46&amp;" "&amp;B46&amp;","</f>
@@ -3094,10 +3246,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">A47&amp;" "&amp;B47&amp;","</f>
@@ -3117,8 +3269,8 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;A35&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_objeto_gasto PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;A35&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_objeto_gasto PRIMARY KEY (id) );</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>140</v>
@@ -3203,17 +3355,17 @@
       </c>
       <c r="B52" s="0" t="str">
         <f aca="false">Sheet2!$B$1</f>
-        <v>numeric(5,0)</v>
+        <v>Numeric(5,0)</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">A52&amp;" "&amp;B52&amp;","</f>
-        <v>control_financiero_codigo numeric(5,0),</v>
+        <v>control_financiero_codigo Numeric(5,0),</v>
       </c>
       <c r="D52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F52" s="0" t="str">
         <f aca="false">D52&amp;" "&amp;E52&amp;","</f>
@@ -3233,10 +3385,10 @@
         <v>control_financiero_descripcion character varying,</v>
       </c>
       <c r="D53" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="F53" s="0" t="str">
         <f aca="false">D53&amp;" "&amp;E53&amp;","</f>
@@ -3255,8 +3407,8 @@
         <v>fecha_vigencia timestamp without time zone,</v>
       </c>
       <c r="F54" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;D40&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_proveedor PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;D40&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_proveedor PRIMARY KEY (id) );</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,15 +3428,15 @@
       <c r="E55" s="1"/>
       <c r="F55" s="2" t="str">
         <f aca="false">"CREATE TABLE "&amp;D55&amp;" ("</f>
-        <v>CREATE TABLE dim_cuentas_bancarias (</v>
+        <v>CREATE TABLE dim_cuenta_bancaria (</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">A56&amp;" "&amp;B56&amp;","</f>
@@ -3303,10 +3455,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">A57&amp;" "&amp;B57&amp;","</f>
@@ -3326,8 +3478,8 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;A49&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_clasificador_control_financiero PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;A49&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_clasificador_control_financiero PRIMARY KEY (id) );</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>147</v>
@@ -3356,7 +3508,7 @@
       </c>
       <c r="F59" s="0" t="str">
         <f aca="false">D59&amp;" "&amp;E59&amp;","</f>
-        <v>banco_abreviatura character varying,</v>
+        <v>banco_simbolo character varying,</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,7 +3526,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E61" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -3387,7 +3539,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D62" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E62" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -3400,7 +3552,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D63" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E63" s="0" t="str">
         <f aca="false">Sheet2!$B$3</f>
@@ -3437,10 +3589,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F66" s="0" t="str">
         <f aca="false">D66&amp;" "&amp;E66&amp;","</f>
@@ -3449,10 +3601,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D67" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="F67" s="0" t="str">
         <f aca="false">D67&amp;" "&amp;E67&amp;","</f>
@@ -3461,8 +3613,8 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="0" t="str">
-        <f aca="false">"CONSTRAINT pk_"&amp;D55&amp;" PRIMARY KEY (id) )"</f>
-        <v>CONSTRAINT pk_dim_cuentas_bancarias PRIMARY KEY (id) )</v>
+        <f aca="false">"CONSTRAINT pk_"&amp;D55&amp;" PRIMARY KEY (id) );"</f>
+        <v>CONSTRAINT pk_dim_cuenta_bancaria PRIMARY KEY (id) );</v>
       </c>
     </row>
   </sheetData>
@@ -3484,7 +3636,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3498,7 +3650,7 @@
       <c r="A1" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3515,7 +3667,7 @@
         <v>155</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>